<commit_message>
Calibrated Ultrasound device for accuracy. Added PWM and Motor to control arm - currently incomplete.
</commit_message>
<xml_diff>
--- a/MouseTrap/References/Port Assignments.xlsx
+++ b/MouseTrap/References/Port Assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M Hanzalah\Documents\Embedded\STM32F103RB\MouseTrap\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3555A195-7CCA-4225-A78C-16893DAFDC37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F7D84B-11D4-41A6-AC0E-FCB9B127D303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17955" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>PA</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Ultrasound Trigger</t>
+  </si>
+  <si>
+    <t>Motor Direction</t>
+  </si>
+  <si>
+    <t>Motor PWM</t>
   </si>
 </sst>
 </file>
@@ -399,12 +405,14 @@
   <dimension ref="B3:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
@@ -467,12 +475,8 @@
       <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="1">
-        <v>34</v>
-      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="L4" s="2">
         <v>0</v>
@@ -491,8 +495,12 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="G5" s="2">
         <v>1</v>
@@ -509,8 +517,12 @@
       <c r="Q5" s="2">
         <v>1</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
+      <c r="R5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="1">
+        <v>31</v>
+      </c>
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -631,9 +643,13 @@
       <c r="G10" s="2">
         <v>6</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>17</v>
+      </c>
       <c r="L10" s="2">
         <v>6</v>
       </c>

</xml_diff>